<commit_message>
Changed code to conform to Gavin's recent changes
Changed instances of mirrorMode == true to be gameLogic.gameMode == 2. Also updated my time to reflect the time spent bug testing group 15's code.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stoned_Darksst\Desktop\Fall 2021\EECS 448\Project 2\EECS-448_Project-2_G11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panda\Desktop\EECS_448\EECS-448_Project-2_G11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3538B8D1-BFFB-4575-AE92-8FA75E29A1A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE957CED-96F6-4239-AA9B-FF3850B51D16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5790" yWindow="720" windowWidth="21600" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +423,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="D5">
         <v>1.5</v>

</xml_diff>

<commit_message>
Updated the Time sheet with our estimate
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbthi\Documents\GitHub\EECS-448_Project-2_G11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakeangus/Documents/School/Fall_2021/EECS_448/EECS-448_Project-2_G11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFF0707-473F-4232-8F01-E32176FD1BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95816AE8-E97F-3645-94B7-07D562F38383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Andrew </t>
   </si>
@@ -46,6 +55,15 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Total Person Hours Estimated:</t>
+  </si>
+  <si>
+    <t>Actual Person Hours:</t>
+  </si>
+  <si>
+    <t>We estimated 100 hours on the last project because we were building it from scratch. Here we estimated less because we're only adding a few features to an already complete project.</t>
   </si>
 </sst>
 </file>
@@ -61,15 +79,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,13 +101,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,128 +404,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="140.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2">
+        <f>SUM(C6:G13)</f>
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
         <v>44472</v>
       </c>
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="E3">
-        <v>0.5</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
         <v>44473</v>
       </c>
-      <c r="C4">
-        <v>0.5</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <v>0.5</v>
-      </c>
-      <c r="F4">
-        <v>0.5</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
         <v>44474</v>
       </c>
-      <c r="D5">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>1.5</v>
       </c>
-      <c r="G5">
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
         <v>44475</v>
       </c>
-      <c r="D6">
+      <c r="D9">
         <v>3.5</v>
       </c>
-      <c r="F6">
+      <c r="F9">
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
         <v>44476</v>
       </c>
-      <c r="D7">
+      <c r="D10">
         <v>3.5</v>
       </c>
-      <c r="E7">
+      <c r="E10">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+      <c r="F10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
         <v>44477</v>
       </c>
-      <c r="D8">
+      <c r="D11">
         <v>4.5</v>
       </c>
-      <c r="E8">
+      <c r="E11">
         <v>4.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
         <v>44478</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
         <v>44479</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>